<commit_message>
updated excel with name
</commit_message>
<xml_diff>
--- a/coursera.xlsx
+++ b/coursera.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mandarjadhav/Desktop/GitHandsOn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9961FBAF-04CD-EB4D-8C3A-27A3D76DBE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6034CAC0-3845-F241-B13B-63029A159E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{C1221AA0-1263-5B4D-B419-DB8145949F17}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Actual Class</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Registration fees</t>
+  </si>
+  <si>
+    <t>Mandar</t>
   </si>
 </sst>
 </file>
@@ -4085,8 +4088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D783A9-0D90-47C4-9834-B37F6EBCAF5E}">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="82" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5019,7 +5022,7 @@
         <v>1.7959183673469388</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>40</v>
       </c>
@@ -5056,7 +5059,7 @@
         <v>1.8265306122448979</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>20</v>
       </c>
@@ -5093,7 +5096,7 @@
         <v>1.8535414165666266</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>38</v>
       </c>
@@ -5130,7 +5133,7 @@
         <v>1.8775510204081634</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>28</v>
       </c>
@@ -5167,7 +5170,7 @@
         <v>1.8990332975295383</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>25</v>
       </c>
@@ -5204,7 +5207,7 @@
         <v>1.9183673469387754</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>6</v>
       </c>
@@ -5241,7 +5244,7 @@
         <v>1.8192419825072885</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>2</v>
       </c>
@@ -5278,7 +5281,7 @@
         <v>1.7291280148423003</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -5315,7 +5318,7 @@
         <v>1.6468500443655725</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>1</v>
       </c>
@@ -5352,7 +5355,7 @@
         <v>1.6734693877551021</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>39</v>
       </c>
@@ -5389,7 +5392,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>4</v>
       </c>
@@ -5426,7 +5429,7 @@
         <v>1.6263736263736264</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>9</v>
       </c>
@@ -5462,8 +5465,11 @@
         <f t="shared" si="3"/>
         <v>1.5600907029478457</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="Q28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>11</v>
       </c>
@@ -5500,7 +5506,7 @@
         <v>1.4985422740524781</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>15</v>
       </c>
@@ -5537,7 +5543,7 @@
         <v>1.441238564391274</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>14</v>
       </c>
@@ -5574,7 +5580,7 @@
         <v>1.3877551020408163</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>32</v>
       </c>

</xml_diff>